<commit_message>
Tidied data further, removed formatting on xlsx file
</commit_message>
<xml_diff>
--- a/data/survey-data_tidy.xlsx
+++ b/data/survey-data_tidy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jihoon William Lee\Documents\GitHub\tfcb-homework01\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA29746-2731-4D4E-8E80-940BC85174D5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAF79BD-F206-4591-BD1B-BE9E6B14B134}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="2025" windowWidth="32250" windowHeight="17295" xr2:uid="{B4165ABB-C019-45E9-AB5B-129EE90C33C2}"/>
+    <workbookView xWindow="2760" yWindow="2010" windowWidth="32250" windowHeight="17295" xr2:uid="{B4165ABB-C019-45E9-AB5B-129EE90C33C2}"/>
   </bookViews>
   <sheets>
     <sheet name="tidy" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="44">
   <si>
     <t>NA</t>
   </si>
@@ -170,7 +170,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
-    <numFmt numFmtId="166" formatCode="yyyymmdd"/>
+    <numFmt numFmtId="165" formatCode="yyyymmdd"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -218,7 +218,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,12 +234,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -374,11 +368,10 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,7 +763,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -814,7 +807,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -838,7 +831,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4861EA6B-64F6-4EE9-BBFE-FEBEFEE3787C}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -861,10 +856,10 @@
       <c r="F1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="24"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
+      <c r="A2" s="25">
         <v>41471</v>
       </c>
       <c r="B2" s="24">
@@ -876,16 +871,16 @@
       <c r="D2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="24" t="s">
         <v>43</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="24"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="23">
+      <c r="A3" s="25">
         <v>41471</v>
       </c>
       <c r="B3" s="24">
@@ -903,10 +898,10 @@
       <c r="F3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="24"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="23">
+      <c r="A4" s="25">
         <v>41471</v>
       </c>
       <c r="B4" s="24">
@@ -915,19 +910,19 @@
       <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="26" t="s">
+      <c r="D4" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>43</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="23">
+      <c r="A5" s="25">
         <v>41471</v>
       </c>
       <c r="B5" s="24">
@@ -936,19 +931,19 @@
       <c r="C5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="26" t="s">
+      <c r="D5" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>43</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="24"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="23">
+      <c r="A6" s="25">
         <v>41473</v>
       </c>
       <c r="B6" s="24">
@@ -957,7 +952,7 @@
       <c r="C6" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="24">
@@ -966,10 +961,10 @@
       <c r="F6" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="24"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="23">
+      <c r="A7" s="25">
         <v>41473</v>
       </c>
       <c r="B7" s="24">
@@ -978,7 +973,7 @@
       <c r="C7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="24" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="24">
@@ -987,10 +982,10 @@
       <c r="F7" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="24"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="23">
+      <c r="A8" s="25">
         <v>41473</v>
       </c>
       <c r="B8" s="24">
@@ -999,19 +994,19 @@
       <c r="C8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="25">
+      <c r="D8" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="24">
         <v>29</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="24"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="23">
+      <c r="A9" s="25">
         <v>41473</v>
       </c>
       <c r="B9" s="24">
@@ -1020,19 +1015,19 @@
       <c r="C9" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="25">
+      <c r="D9" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="24">
         <v>37</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="24"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="23">
+      <c r="A10" s="25">
         <v>41505</v>
       </c>
       <c r="B10" s="24">
@@ -1041,19 +1036,19 @@
       <c r="C10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="25">
+      <c r="D10" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="24">
         <v>52</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="24"/>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="23">
+      <c r="A11" s="25">
         <v>41564</v>
       </c>
       <c r="B11" s="24">
@@ -1062,19 +1057,19 @@
       <c r="C11" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="25">
+      <c r="D11" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="24">
         <v>33</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="24"/>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="23">
+      <c r="A12" s="25">
         <v>41564</v>
       </c>
       <c r="B12" s="24">
@@ -1083,19 +1078,19 @@
       <c r="C12" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="25">
+      <c r="D12" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="24">
         <v>50</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="24"/>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="23">
+      <c r="A13" s="25">
         <v>41618</v>
       </c>
       <c r="B13" s="24">
@@ -1104,19 +1099,19 @@
       <c r="C13" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="25">
+      <c r="D13" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="24">
         <v>40</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="24"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="23">
+      <c r="A14" s="25">
         <v>41618</v>
       </c>
       <c r="B14" s="24">
@@ -1125,19 +1120,19 @@
       <c r="C14" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="25">
+      <c r="D14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="24">
         <v>45</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="24"/>
+      <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="23">
+      <c r="A15" s="25">
         <v>41619</v>
       </c>
       <c r="B15" s="24">
@@ -1146,19 +1141,19 @@
       <c r="C15" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="25">
+      <c r="D15" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="24">
         <v>41</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="24"/>
+      <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="23">
+      <c r="A16" s="25">
         <v>41590</v>
       </c>
       <c r="B16" s="24">
@@ -1167,19 +1162,19 @@
       <c r="C16" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="25">
+      <c r="D16" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="24">
         <v>117</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="24"/>
+      <c r="G16" s="23"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="23">
+      <c r="A17" s="25">
         <v>41591</v>
       </c>
       <c r="B17" s="24">
@@ -1188,19 +1183,19 @@
       <c r="C17" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="25">
+      <c r="D17" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="24">
         <v>126</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="24"/>
+      <c r="G17" s="23"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="23">
+      <c r="A18" s="25">
         <v>41591</v>
       </c>
       <c r="B18" s="24">
@@ -1209,19 +1204,19 @@
       <c r="C18" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="25">
+      <c r="D18" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="24">
         <v>132</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="24"/>
+      <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="23">
+      <c r="A19" s="25">
         <v>41591</v>
       </c>
       <c r="B19" s="24">
@@ -1230,19 +1225,19 @@
       <c r="C19" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="25">
+      <c r="D19" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="24">
         <v>113</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="24"/>
+      <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="23">
+      <c r="A20" s="25">
         <v>41591</v>
       </c>
       <c r="B20" s="24">
@@ -1251,19 +1246,19 @@
       <c r="C20" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="25">
+      <c r="D20" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="24">
         <v>122</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="24"/>
+      <c r="G20" s="23"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="23">
+      <c r="A21" s="25">
         <v>41591</v>
       </c>
       <c r="B21" s="24">
@@ -1272,19 +1267,19 @@
       <c r="C21" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="25">
+      <c r="D21" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="24">
         <v>107</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="24"/>
+      <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="23">
+      <c r="A22" s="25">
         <v>41591</v>
       </c>
       <c r="B22" s="24">
@@ -1293,152 +1288,154 @@
       <c r="C22" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="25">
+      <c r="D22" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="24">
         <v>115</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="24"/>
+      <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="23">
+      <c r="A23" s="25">
         <v>41648</v>
       </c>
-      <c r="B23" s="25">
+      <c r="B23" s="24">
         <v>1</v>
       </c>
       <c r="C23" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="25">
+      <c r="D23" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="24">
         <v>40</v>
       </c>
       <c r="F23" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="24"/>
+      <c r="G23" s="23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="23">
+      <c r="A24" s="25">
         <v>41648</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24" s="24">
         <v>1</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="25">
+      <c r="D24" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="24">
         <v>36</v>
       </c>
       <c r="F24" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="24"/>
+      <c r="G24" s="23"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="23">
+      <c r="A25" s="25">
         <v>41711</v>
       </c>
-      <c r="B25" s="25">
+      <c r="B25" s="24">
         <v>1</v>
       </c>
       <c r="C25" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="25">
+      <c r="D25" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="24">
         <v>51</v>
       </c>
       <c r="F25" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="24"/>
+      <c r="G25" s="23"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="23">
+      <c r="A26" s="25">
         <v>41711</v>
       </c>
-      <c r="B26" s="25">
+      <c r="B26" s="24">
         <v>1</v>
       </c>
       <c r="C26" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="25">
+      <c r="D26" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="24">
         <v>44</v>
       </c>
       <c r="F26" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G26" s="24"/>
+      <c r="G26" s="23"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="23">
+      <c r="A27" s="25">
         <v>41711</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="24">
         <v>1</v>
       </c>
       <c r="C27" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="25">
+      <c r="D27" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="24">
         <v>146</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G27" s="24"/>
+      <c r="G27" s="23"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="23">
+      <c r="A28" s="25">
         <v>41647</v>
       </c>
-      <c r="B28" s="25">
+      <c r="B28" s="24">
         <v>2</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="26" t="s">
+      <c r="D28" s="24" t="s">
         <v>43</v>
       </c>
+      <c r="E28" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="F28" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G28" s="24"/>
+      <c r="G28" s="23"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="23">
+      <c r="A29" s="25">
         <v>41647</v>
       </c>
-      <c r="B29" s="25">
+      <c r="B29" s="24">
         <v>2</v>
       </c>
       <c r="C29" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="24" t="s">
         <v>1</v>
       </c>
       <c r="E29" s="24">
@@ -1447,19 +1444,19 @@
       <c r="F29" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G29" s="24"/>
+      <c r="G29" s="23"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="23">
+      <c r="A30" s="25">
         <v>41647</v>
       </c>
-      <c r="B30" s="25">
+      <c r="B30" s="24">
         <v>2</v>
       </c>
       <c r="C30" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="24">
@@ -1468,19 +1465,19 @@
       <c r="F30" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="24"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="23">
+      <c r="A31" s="25">
         <v>41647</v>
       </c>
-      <c r="B31" s="25">
+      <c r="B31" s="24">
         <v>2</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="25" t="s">
+      <c r="D31" s="24" t="s">
         <v>1</v>
       </c>
       <c r="E31" s="24">
@@ -1489,38 +1486,40 @@
       <c r="F31" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G31" s="24"/>
+      <c r="G31" s="23"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="23">
+      <c r="A32" s="25">
         <v>41647</v>
       </c>
-      <c r="B32" s="25">
+      <c r="B32" s="24">
         <v>2</v>
       </c>
       <c r="C32" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="26" t="s">
+      <c r="D32" s="24" t="s">
         <v>43</v>
       </c>
+      <c r="E32" s="24" t="s">
+        <v>43</v>
+      </c>
       <c r="F32" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G32" s="24"/>
+      <c r="G32" s="23"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="23">
+      <c r="A33" s="25">
         <v>41647</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B33" s="24">
         <v>2</v>
       </c>
       <c r="C33" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="25" t="s">
+      <c r="D33" s="24" t="s">
         <v>1</v>
       </c>
       <c r="E33" s="24">
@@ -1529,38 +1528,40 @@
       <c r="F33" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="G33" s="24"/>
+      <c r="G33" s="23"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="23">
+      <c r="A34" s="25">
         <v>41647</v>
       </c>
-      <c r="B34" s="25">
+      <c r="B34" s="24">
         <v>2</v>
       </c>
       <c r="C34" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="24"/>
-      <c r="E34" s="26" t="s">
+      <c r="D34" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="F34" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G34" s="24"/>
+      <c r="E34" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" s="23"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="23">
+      <c r="A35" s="25">
         <v>41688</v>
       </c>
-      <c r="B35" s="25">
+      <c r="B35" s="24">
         <v>2</v>
       </c>
       <c r="C35" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="24" t="s">
         <v>1</v>
       </c>
       <c r="E35" s="24">
@@ -1569,299 +1570,301 @@
       <c r="F35" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="G35" s="24"/>
+      <c r="G35" s="23"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="23">
+      <c r="A36" s="25">
         <v>41688</v>
       </c>
-      <c r="B36" s="25">
+      <c r="B36" s="24">
         <v>2</v>
       </c>
       <c r="C36" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D36" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="24">
         <v>7</v>
       </c>
-      <c r="F36" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G36" s="24"/>
+      <c r="F36" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G36" s="23"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="23">
+      <c r="A37" s="25">
         <v>41688</v>
       </c>
-      <c r="B37" s="25">
+      <c r="B37" s="24">
         <v>2</v>
       </c>
       <c r="C37" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="25" t="s">
+      <c r="D37" s="24" t="s">
         <v>1</v>
       </c>
       <c r="E37" s="24">
         <v>52</v>
       </c>
-      <c r="F37" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G37" s="24"/>
+      <c r="F37" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G37" s="23"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="23">
+      <c r="A38" s="25">
         <v>41709</v>
       </c>
-      <c r="B38" s="25">
+      <c r="B38" s="24">
         <v>3</v>
       </c>
       <c r="C38" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="25" t="s">
+      <c r="D38" s="24" t="s">
         <v>1</v>
       </c>
       <c r="E38" s="24">
         <v>8</v>
       </c>
-      <c r="F38" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G38" s="24"/>
+      <c r="F38" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" s="23"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="23">
+      <c r="A39" s="25">
         <v>41737</v>
       </c>
-      <c r="B39" s="25">
+      <c r="B39" s="24">
         <v>3</v>
       </c>
       <c r="C39" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D39" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" s="26" t="s">
+      <c r="D39" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G39" s="24"/>
+      <c r="F39" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G39" s="23"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="23">
+      <c r="A40" s="25">
         <v>41765</v>
       </c>
-      <c r="B40" s="25">
-        <v>3</v>
-      </c>
-      <c r="C40" s="26" t="s">
+      <c r="B40" s="24">
+        <v>3</v>
+      </c>
+      <c r="C40" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="24"/>
-      <c r="E40" s="26" t="s">
+      <c r="D40" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="F40" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G40" s="24"/>
+      <c r="E40" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="23">
+      <c r="A41" s="25">
         <v>41777</v>
       </c>
-      <c r="B41" s="25">
+      <c r="B41" s="24">
         <v>3</v>
       </c>
       <c r="C41" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D41" s="25" t="s">
+      <c r="D41" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="24">
         <v>182</v>
       </c>
-      <c r="F41" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G41" s="24"/>
+      <c r="F41" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="23">
+      <c r="A42" s="25">
         <v>41799</v>
       </c>
-      <c r="B42" s="25">
+      <c r="B42" s="24">
         <v>3</v>
       </c>
       <c r="C42" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="25" t="s">
+      <c r="D42" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E42" s="24">
         <v>29</v>
       </c>
-      <c r="F42" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G42" s="24"/>
+      <c r="F42" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G42" s="23"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="23">
+      <c r="A43" s="25">
         <v>41828</v>
       </c>
-      <c r="B43" s="25">
+      <c r="B43" s="24">
         <v>3</v>
       </c>
       <c r="C43" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D43" s="25" t="s">
+      <c r="D43" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E43" s="24">
         <v>115</v>
       </c>
-      <c r="F43" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G43" s="24"/>
+      <c r="F43" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G43" s="23"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="23">
+      <c r="A44" s="25">
         <v>41828</v>
       </c>
-      <c r="B44" s="25">
+      <c r="B44" s="24">
         <v>3</v>
       </c>
       <c r="C44" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D44" s="25" t="s">
+      <c r="D44" s="24" t="s">
         <v>1</v>
       </c>
       <c r="E44" s="24">
         <v>190</v>
       </c>
-      <c r="F44" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G44" s="24"/>
+      <c r="F44" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G44" s="23"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="23">
+      <c r="A45" s="25">
         <v>28498</v>
       </c>
-      <c r="B45" s="25">
+      <c r="B45" s="24">
         <v>4</v>
       </c>
       <c r="C45" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="25" t="s">
+      <c r="D45" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="24">
         <v>37</v>
       </c>
-      <c r="F45" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G45" s="24"/>
+      <c r="F45" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G45" s="23"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="23">
+      <c r="A46" s="25">
         <v>28498</v>
       </c>
-      <c r="B46" s="25">
+      <c r="B46" s="24">
         <v>4</v>
       </c>
       <c r="C46" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E46" s="26" t="s">
+      <c r="D46" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="F46" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G46" s="24"/>
+      <c r="F46" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G46" s="23"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="23">
+      <c r="A47" s="25">
         <v>28498</v>
       </c>
-      <c r="B47" s="25">
+      <c r="B47" s="24">
         <v>4</v>
       </c>
       <c r="C47" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D47" s="25" t="s">
+      <c r="D47" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E47" s="24">
         <v>48</v>
       </c>
-      <c r="F47" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G47" s="24"/>
+      <c r="F47" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47" s="23"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="23">
+      <c r="A48" s="25">
         <v>28498</v>
       </c>
-      <c r="B48" s="25">
+      <c r="B48" s="24">
         <v>4</v>
       </c>
       <c r="C48" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="25" t="s">
+      <c r="D48" s="24" t="s">
         <v>1</v>
       </c>
       <c r="E48" s="24">
         <v>52</v>
       </c>
-      <c r="F48" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G48" s="24"/>
+      <c r="F48" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G48" s="23"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="23">
+      <c r="A49" s="25">
         <v>28498</v>
       </c>
-      <c r="B49" s="25">
+      <c r="B49" s="24">
         <v>4</v>
       </c>
       <c r="C49" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="24" t="s">
         <v>1</v>
       </c>
       <c r="E49" s="24">
         <v>35</v>
       </c>
-      <c r="F49" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G49" s="24"/>
+      <c r="F49" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G49" s="23"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="22"/>

</xml_diff>